<commit_message>
complete run of TOD-C schoolage norms, both age and grades, with zero scores
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODC_final_gr1_12_10.28.21_fornorms/lem_sum-raw-ss-lookup-tabbed-age.xlsx
+++ b/OUTPUT-FILES/NORMS/TODC_final_gr1_12_10.28.21_fornorms/lem_sum-raw-ss-lookup-tabbed-age.xlsx
@@ -370,7 +370,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -390,71 +390,71 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>130</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>130</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>130</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>130</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>130</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -542,9 +542,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -555,7 +563,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -575,95 +583,95 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>130</v>
@@ -671,7 +679,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>130</v>
@@ -679,7 +687,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -687,7 +695,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -695,7 +703,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -703,7 +711,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -711,7 +719,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -719,7 +727,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -727,9 +735,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -740,7 +756,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -760,95 +776,95 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>130</v>
@@ -856,7 +872,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>130</v>
@@ -864,7 +880,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -872,7 +888,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -880,7 +896,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -888,7 +904,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -896,7 +912,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -904,7 +920,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -912,9 +928,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -925,7 +949,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -945,103 +969,103 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>130</v>
@@ -1049,7 +1073,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -1057,7 +1081,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -1065,7 +1089,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -1073,7 +1097,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -1081,7 +1105,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -1089,7 +1113,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -1097,9 +1121,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -1110,7 +1142,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1130,103 +1162,103 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>130</v>
@@ -1234,7 +1266,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -1242,7 +1274,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -1250,7 +1282,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -1258,7 +1290,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -1266,7 +1298,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -1274,7 +1306,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -1282,9 +1314,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -1295,7 +1335,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1315,103 +1355,103 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>130</v>
@@ -1419,7 +1459,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -1427,7 +1467,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -1435,7 +1475,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -1443,7 +1483,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -1451,7 +1491,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -1459,7 +1499,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -1467,9 +1507,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -1480,7 +1528,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1500,111 +1548,111 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -1612,7 +1660,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -1620,7 +1668,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -1628,7 +1676,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -1636,7 +1684,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -1644,7 +1692,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -1652,9 +1700,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -1665,7 +1721,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1685,111 +1741,111 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -1797,7 +1853,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -1805,7 +1861,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -1813,7 +1869,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -1821,7 +1877,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -1829,7 +1885,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -1837,9 +1893,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -1850,7 +1914,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1870,111 +1934,111 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -1982,7 +2046,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -1990,7 +2054,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -1998,7 +2062,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -2006,7 +2070,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -2014,7 +2078,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -2022,9 +2086,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -2035,7 +2107,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2055,119 +2127,119 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -2175,7 +2247,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -2183,7 +2255,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -2191,7 +2263,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -2199,7 +2271,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -2207,9 +2279,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -2220,7 +2300,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2240,127 +2320,127 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -2368,7 +2448,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -2376,7 +2456,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -2384,7 +2464,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -2392,9 +2472,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -2405,7 +2493,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2425,79 +2513,79 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>130</v>
@@ -2505,7 +2593,7 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>130</v>
@@ -2513,7 +2601,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>130</v>
@@ -2521,7 +2609,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>130</v>
@@ -2529,7 +2617,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -2537,7 +2625,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -2545,7 +2633,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -2553,7 +2641,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -2561,7 +2649,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -2569,7 +2657,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -2577,9 +2665,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -2590,7 +2686,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2610,127 +2706,127 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -2738,7 +2834,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -2746,7 +2842,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -2754,7 +2850,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -2762,9 +2858,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -2775,7 +2879,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2795,79 +2899,79 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>130</v>
@@ -2875,7 +2979,7 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>130</v>
@@ -2883,7 +2987,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>130</v>
@@ -2891,7 +2995,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>130</v>
@@ -2899,7 +3003,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -2907,7 +3011,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -2915,7 +3019,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -2923,7 +3027,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -2931,7 +3035,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -2939,7 +3043,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -2947,9 +3051,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -2960,7 +3072,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2980,79 +3092,79 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>130</v>
@@ -3060,7 +3172,7 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>130</v>
@@ -3068,7 +3180,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>130</v>
@@ -3076,7 +3188,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>130</v>
@@ -3084,7 +3196,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -3092,7 +3204,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -3100,7 +3212,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -3108,7 +3220,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -3116,7 +3228,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -3124,7 +3236,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -3132,9 +3244,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -3145,7 +3265,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3165,79 +3285,79 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>130</v>
@@ -3245,7 +3365,7 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>130</v>
@@ -3253,7 +3373,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>130</v>
@@ -3261,7 +3381,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>130</v>
@@ -3269,7 +3389,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -3277,7 +3397,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -3285,7 +3405,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -3293,7 +3413,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -3301,7 +3421,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -3309,7 +3429,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -3317,9 +3437,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -3330,7 +3458,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3350,87 +3478,87 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>130</v>
@@ -3438,7 +3566,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>130</v>
@@ -3446,7 +3574,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>130</v>
@@ -3454,7 +3582,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -3462,7 +3590,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -3470,7 +3598,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -3478,7 +3606,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -3486,7 +3614,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -3494,7 +3622,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -3502,9 +3630,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -3515,7 +3651,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3535,87 +3671,87 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>130</v>
@@ -3623,7 +3759,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>130</v>
@@ -3631,7 +3767,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>130</v>
@@ -3639,7 +3775,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -3647,7 +3783,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -3655,7 +3791,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -3663,7 +3799,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -3671,7 +3807,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -3679,7 +3815,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -3687,9 +3823,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -3700,7 +3844,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3720,87 +3864,87 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>130</v>
@@ -3808,7 +3952,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>130</v>
@@ -3816,7 +3960,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>130</v>
@@ -3824,7 +3968,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -3832,7 +3976,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -3840,7 +3984,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -3848,7 +3992,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -3856,7 +4000,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -3864,7 +4008,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -3872,9 +4016,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -3885,7 +4037,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3905,95 +4057,95 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>130</v>
@@ -4001,7 +4153,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>130</v>
@@ -4009,7 +4161,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -4017,7 +4169,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>130</v>
@@ -4025,7 +4177,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -4033,7 +4185,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -4041,7 +4193,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -4049,7 +4201,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -4057,9 +4209,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>

</xml_diff>